<commit_message>
Descripción ampliada de la tercera imagen
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado08/guion07/SolicitudGrafica_CN_08_07_CO_REC20.xlsx
+++ b/fuentes/contenidos/grado08/guion07/SolicitudGrafica_CN_08_07_CO_REC20.xlsx
@@ -606,13 +606,14 @@
     <t>Ilustración</t>
   </si>
   <si>
-    <t>Cuadros con cruces de mosas</t>
-  </si>
-  <si>
-    <t>Se debe ilustrar la imagen anterior. Son dos imágenes, que se encuentran en la página web del enlace. Allí hay varias imágenes, tomar sólo las dos que aparecen en la ilustración de arriba. Se ponen las dos imágenes en una, sin modificaciones, excepto porque se marcan como A y B (justo como en la imagen de arriba).</t>
-  </si>
-  <si>
     <t>Microscopio con cromosomas X en el fondo</t>
+  </si>
+  <si>
+    <t>Cuadros con cruces de moscas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Se debe ilustrar la imagen anterior. Son dos imágenes, que se encuentran en la página web del enlace. Allí hay varias imágenes, tomar sólo las dos que aparecen en la ilustración de arriba. Se ponen las dos imágenes en una, sin modificaciones, excepto porque se marcan como A y B. Debe notarse que las letras y flechas en verde sin aclaraciones, y NO deben quedar en la imagen para poner en el recurso. Las X dentro de los cuadros parecen tener comillas, pero en realidad son letras en superíndices. Las letras y flechas verdes indican cómo deben quedar esos superíndices. Supongo que habrá que hacer la imagen más grande para que las letras se noten. O, si es necesario, entregar dos imágenes diferentes y yo hago una diapositiva extra. En ese caso no se marcarían como A y B. Hay un cambio más: las dos moscas de arriba de la primera imagen dicen "Hembra de ojos rojos (F1)" y "Macho original de ojos blancos". Cambiar esos textos por, respectivamente, "Hembra de ojos rojos" y "Macho de ojos blancos". También hay que quitar una P que vuela, y una F. En la imagen que adjunto esas letras están tachadas, así que creo será fácil ubicarlas.</t>
   </si>
 </sst>
 </file>
@@ -1778,19 +1779,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>118824</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>5730643</xdr:colOff>
+      <xdr:colOff>5862553</xdr:colOff>
       <xdr:row>11</xdr:row>
-      <xdr:rowOff>2775454</xdr:rowOff>
+      <xdr:rowOff>2711421</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="2 Imagen"/>
+        <xdr:cNvPr id="2" name="1 Imagen"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1803,8 +1804,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="16449675" y="2595324"/>
-          <a:ext cx="5644918" cy="2650280"/>
+          <a:off x="16630650" y="2800350"/>
+          <a:ext cx="5614903" cy="2597121"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2433,9 +2434,9 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:P108"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="140" workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J10" sqref="J10"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" zoomScalePageLayoutView="140" workbookViewId="0">
+      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -2758,7 +2759,7 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J10" s="63" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="K10" s="64"/>
       <c r="O10" s="2" t="str">
@@ -2809,7 +2810,7 @@
         <v>M101</v>
       </c>
     </row>
-    <row r="12" spans="1:16" s="11" customFormat="1" ht="291.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="11" customFormat="1" ht="370.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>IMG03</v>
@@ -2844,10 +2845,10 @@
         <v>800 x 458 px</v>
       </c>
       <c r="J12" s="64" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="K12" s="64" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="O12" s="2" t="str">
         <f>'Definición técnica de imagenes'!A18</f>

</xml_diff>